<commit_message>
Generate nullables on root classes only if there are null values
</commit_message>
<xml_diff>
--- a/SampleTests/ExcelTests/Misc.xlsx
+++ b/SampleTests/ExcelTests/Misc.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cburge\Documents\repos\customer-tests-excel\SampleTests\ExcelTests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEB405BD-7A8B-42C8-BB61-DCEE0B6FA521}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBF1DF17-118E-4DD9-BC1B-095A288A88AE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{93574C7F-CD34-4A26-A791-2CAAC18DAAC8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{93574C7F-CD34-4A26-A791-2CAAC18DAAC8}"/>
   </bookViews>
   <sheets>
     <sheet name="Functions" sheetId="1" r:id="rId1"/>
     <sheet name="Underscores" sheetId="2" r:id="rId2"/>
     <sheet name="CustomProperties" sheetId="3" r:id="rId3"/>
     <sheet name="NullObjects" sheetId="4" r:id="rId4"/>
+    <sheet name="RootNullablePrimitives" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="50">
   <si>
     <t>Specification</t>
   </si>
@@ -97,66 +98,97 @@
   </si>
   <si>
     <t>Do Nothing</t>
+  </si>
+  <si>
+    <t>Then</t>
+  </si>
+  <si>
+    <t>Table_Property table of</t>
+  </si>
+  <si>
+    <t>Underscores in names are converted to underscores in C#, it just checks that the code compiles, and doesn't contain any meaningful setup or assertions.
+Classes that have non matching properties are still generated, and rely on custom code in a partial class to provide the implementation.</t>
+  </si>
+  <si>
+    <t>Classes that have non matching properties are still generated, and rely on custom code in a partial class to provide the implementation.</t>
+  </si>
+  <si>
+    <t>UnmatchedClass</t>
+  </si>
+  <si>
+    <t>ClassWithCustomProperty</t>
+  </si>
+  <si>
+    <t>ClassWithCustomProperty of</t>
+  </si>
+  <si>
+    <t>CustomInt of</t>
+  </si>
+  <si>
+    <t>Nulls can be passed as objects</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>Null can be passed to something that expects an object</t>
+  </si>
+  <si>
+    <t>HasObjectProperty</t>
+  </si>
+  <si>
+    <t>HasObjectProperty of</t>
+  </si>
+  <si>
+    <t>Anything of</t>
+  </si>
+  <si>
+    <t>NullObjectTester</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>RootObject</t>
+  </si>
+  <si>
+    <t>NullableInt of</t>
+  </si>
+  <si>
+    <t>Nullability is calculated from values for generated root setup classes</t>
+  </si>
+  <si>
+    <t>When generating most classes, the framework will search for matching C# classes and determine the type from these</t>
+  </si>
+  <si>
+    <t>However, root classes have no matching C# class, so the framework must work out / guess the type from the supplied values</t>
+  </si>
+  <si>
+    <t>There is a number and a null value for this property, so its type will be Double?</t>
+  </si>
+  <si>
+    <t>The root class is the first one in a test, following "Given a" ("RootObject" in this tab)</t>
+  </si>
+  <si>
+    <t>There is just a number value for this property, so it's type will be Double</t>
+  </si>
+  <si>
+    <t>NullableString of</t>
+  </si>
+  <si>
+    <t>cedd</t>
+  </si>
+  <si>
+    <t>Strings are inherently nullable, so the type for this is String, even though it has text and null values</t>
+  </si>
+  <si>
+    <t>Number of</t>
   </si>
   <si>
     <t>Functions can be set up, as well as properties
 If a class contains a function, then the framework will not be able to create a setup class for it (as they use interfaces from your system under test, whereas functions imply that a concrete object is being used).
-This isn't a problem, but means you will probably need to write the setup class manually.</t>
-  </si>
-  <si>
-    <t>Then</t>
-  </si>
-  <si>
-    <t>Table_Property table of</t>
-  </si>
-  <si>
-    <t>Underscores in names are converted to underscores in C#, it just checks that the code compiles, and doesn't contain any meaningful setup or assertions.
-Classes that have non matching properties are still generated, and rely on custom code in a partial class to provide the implementation.</t>
-  </si>
-  <si>
-    <t>Classes that have non matching properties are still generated, and rely on custom code in a partial class to provide the implementation.</t>
-  </si>
-  <si>
-    <t>UnmatchedClass</t>
-  </si>
-  <si>
-    <t>ClassWithCustomProperty</t>
-  </si>
-  <si>
-    <t>ClassWithCustomProperty of</t>
-  </si>
-  <si>
-    <t>CustomInt of</t>
-  </si>
-  <si>
-    <t>Nulls can be passed as objects</t>
-  </si>
-  <si>
-    <t>null</t>
-  </si>
-  <si>
-    <t>Null can be passed to something that expects an object</t>
-  </si>
-  <si>
-    <t>HasObjectProperty</t>
-  </si>
-  <si>
-    <t>HasObjectProperty of</t>
-  </si>
-  <si>
-    <t>Anything of</t>
-  </si>
-  <si>
-    <t>NullObjectTester</t>
-  </si>
-  <si>
-    <t>Anything</t>
-  </si>
-  <si>
-    <t>AnInteger of</t>
-  </si>
-  <si>
-    <t>This isn't required, but it means that when generating the setup classes, we know what the type is. If there were only ever null values for an object, you would need to add a function to set this up in an associated partial class</t>
+This isn't a problem, but means you will probably need to write the setup class manually.
+Only functions with no parameters are supported at the moment</t>
   </si>
 </sst>
 </file>
@@ -205,7 +237,110 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="234">
+  <dxfs count="247">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2372,7 +2507,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1389079D-C9FD-4AFA-AFB3-2F9AFFAD165C}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2387,7 +2524,7 @@
     <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2401,7 +2538,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>21</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -2435,7 +2572,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -2451,49 +2588,49 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="cellIs" dxfId="233" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="246" priority="4" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="232" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="245" priority="5" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="231" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="244" priority="6" operator="equal">
       <formula>"Given a"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="230" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="243" priority="7" operator="equal">
       <formula>"Specification"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="229" priority="8" operator="beginsWith" text="With Properties">
+    <cfRule type="beginsWith" dxfId="242" priority="8" operator="beginsWith" text="With Properties">
       <formula>LEFT(A1,LEN("With Properties"))="With Properties"</formula>
     </cfRule>
-    <cfRule type="endsWith" dxfId="228" priority="9" operator="endsWith" text=" table of">
+    <cfRule type="endsWith" dxfId="241" priority="9" operator="endsWith" text=" table of">
       <formula>RIGHT(A1,LEN(" table of"))=" table of"</formula>
     </cfRule>
-    <cfRule type="endsWith" dxfId="227" priority="10" operator="endsWith" text=" of">
+    <cfRule type="endsWith" dxfId="240" priority="10" operator="endsWith" text=" of">
       <formula>RIGHT(A1,LEN(" of"))=" of"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="226" priority="11">
+    <cfRule type="expression" dxfId="239" priority="11">
       <formula>AND((RIGHT(A1048576, 3) = " of"), A2 = "With Properties")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="225" priority="12">
+    <cfRule type="expression" dxfId="238" priority="12">
       <formula>AND(RIGHT(XFD1, 3) = " of", A2 = "With Properties")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="notContainsBlanks" dxfId="224" priority="13">
+    <cfRule type="notContainsBlanks" dxfId="237" priority="13">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="cellIs" dxfId="223" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="236" priority="2" operator="equal">
       <formula>"PercentagePrecision"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="222" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="235" priority="3" operator="equal">
       <formula>"="</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="cellIs" dxfId="221" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="234" priority="1" operator="equal">
       <formula>"StringFormat"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2537,7 +2674,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -2563,7 +2700,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>10</v>
@@ -2615,7 +2752,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
@@ -2634,378 +2771,378 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A8:C8 A9:D9 A10:C10 C10:XFD11 E8:XFD9 A1:XFD7 A12:XFD1048576">
-    <cfRule type="cellIs" dxfId="220" priority="95" operator="equal">
+    <cfRule type="cellIs" dxfId="233" priority="95" operator="equal">
       <formula>"Assert"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="219" priority="96" operator="equal">
+    <cfRule type="cellIs" dxfId="232" priority="96" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="218" priority="97" operator="equal">
+    <cfRule type="cellIs" dxfId="231" priority="97" operator="equal">
       <formula>"Given a"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="217" priority="98" operator="equal">
+    <cfRule type="cellIs" dxfId="230" priority="98" operator="equal">
       <formula>"Specification"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="216" priority="99" operator="beginsWith" text="With Properties">
+    <cfRule type="beginsWith" dxfId="229" priority="99" operator="beginsWith" text="With Properties">
       <formula>LEFT(A1,LEN("With Properties"))="With Properties"</formula>
     </cfRule>
-    <cfRule type="endsWith" dxfId="215" priority="100" operator="endsWith" text=" table of">
+    <cfRule type="endsWith" dxfId="228" priority="100" operator="endsWith" text=" table of">
       <formula>RIGHT(A1,LEN(" table of"))=" table of"</formula>
     </cfRule>
-    <cfRule type="endsWith" dxfId="214" priority="101" operator="endsWith" text=" of">
+    <cfRule type="endsWith" dxfId="227" priority="101" operator="endsWith" text=" of">
       <formula>RIGHT(A1,LEN(" of"))=" of"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="213" priority="102">
+    <cfRule type="expression" dxfId="226" priority="102">
       <formula>AND((RIGHT(A1048576, 3) = " of"), A2 = "With Properties")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="212" priority="103">
+    <cfRule type="expression" dxfId="225" priority="103">
       <formula>AND(RIGHT(XFD1, 3) = " of", A2 = "With Properties")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8:C8 A9:D9 A10:C10 C10:XFD11 E8:XFD9 A1:XFD7 A12:XFD1048576">
-    <cfRule type="notContainsBlanks" dxfId="211" priority="104">
+    <cfRule type="notContainsBlanks" dxfId="224" priority="104">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8:C8 A9:D9 A10:C10 C10:XFD11 E8:XFD9 A1:XFD7 A12:XFD1048576">
-    <cfRule type="cellIs" dxfId="210" priority="93" operator="equal">
+    <cfRule type="cellIs" dxfId="223" priority="93" operator="equal">
       <formula>"PercentagePrecision"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="209" priority="94" operator="equal">
+    <cfRule type="cellIs" dxfId="222" priority="94" operator="equal">
       <formula>"="</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8:C8 A9:D9 A10:C10 C10:XFD11 E8:XFD9 A1:XFD7 A12:XFD1048576">
-    <cfRule type="cellIs" dxfId="208" priority="92" operator="equal">
+    <cfRule type="cellIs" dxfId="221" priority="92" operator="equal">
       <formula>"StringFormat"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9">
-    <cfRule type="cellIs" dxfId="207" priority="82" operator="equal">
+    <cfRule type="cellIs" dxfId="220" priority="82" operator="equal">
       <formula>"Assert"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="206" priority="83" operator="equal">
+    <cfRule type="cellIs" dxfId="219" priority="83" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="205" priority="84" operator="equal">
+    <cfRule type="cellIs" dxfId="218" priority="84" operator="equal">
       <formula>"Given a"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="204" priority="85" operator="equal">
+    <cfRule type="cellIs" dxfId="217" priority="85" operator="equal">
       <formula>"Specification"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="203" priority="86" operator="beginsWith" text="With Properties">
+    <cfRule type="beginsWith" dxfId="216" priority="86" operator="beginsWith" text="With Properties">
       <formula>LEFT(D9,LEN("With Properties"))="With Properties"</formula>
     </cfRule>
-    <cfRule type="endsWith" dxfId="202" priority="87" operator="endsWith" text=" table of">
+    <cfRule type="endsWith" dxfId="215" priority="87" operator="endsWith" text=" table of">
       <formula>RIGHT(D9,LEN(" table of"))=" table of"</formula>
     </cfRule>
-    <cfRule type="endsWith" dxfId="201" priority="88" operator="endsWith" text=" of">
+    <cfRule type="endsWith" dxfId="214" priority="88" operator="endsWith" text=" of">
       <formula>RIGHT(D9,LEN(" of"))=" of"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="200" priority="89">
+    <cfRule type="expression" dxfId="213" priority="89">
       <formula>AND((RIGHT(D8, 3) = " of"), D10 = "With Properties")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="199" priority="90">
+    <cfRule type="expression" dxfId="212" priority="90">
       <formula>AND(RIGHT(C9, 3) = " of", D10 = "With Properties")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9">
-    <cfRule type="notContainsBlanks" dxfId="198" priority="91">
+    <cfRule type="notContainsBlanks" dxfId="211" priority="91">
       <formula>LEN(TRIM(D9))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9">
-    <cfRule type="cellIs" dxfId="197" priority="80" operator="equal">
+    <cfRule type="cellIs" dxfId="210" priority="80" operator="equal">
       <formula>"PercentagePrecision"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="196" priority="81" operator="equal">
+    <cfRule type="cellIs" dxfId="209" priority="81" operator="equal">
       <formula>"="</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9">
-    <cfRule type="cellIs" dxfId="195" priority="79" operator="equal">
+    <cfRule type="cellIs" dxfId="208" priority="79" operator="equal">
       <formula>"StringFormat"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A9:B13">
-    <cfRule type="cellIs" dxfId="194" priority="69" operator="equal">
+    <cfRule type="cellIs" dxfId="207" priority="69" operator="equal">
       <formula>"Assert"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="193" priority="70" operator="equal">
+    <cfRule type="cellIs" dxfId="206" priority="70" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="192" priority="71" operator="equal">
+    <cfRule type="cellIs" dxfId="205" priority="71" operator="equal">
       <formula>"Given a"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="191" priority="72" operator="equal">
+    <cfRule type="cellIs" dxfId="204" priority="72" operator="equal">
       <formula>"Specification"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="190" priority="73" operator="beginsWith" text="With Properties">
+    <cfRule type="beginsWith" dxfId="203" priority="73" operator="beginsWith" text="With Properties">
       <formula>LEFT(A9,LEN("With Properties"))="With Properties"</formula>
     </cfRule>
-    <cfRule type="endsWith" dxfId="189" priority="74" operator="endsWith" text=" table of">
+    <cfRule type="endsWith" dxfId="202" priority="74" operator="endsWith" text=" table of">
       <formula>RIGHT(A9,LEN(" table of"))=" table of"</formula>
     </cfRule>
-    <cfRule type="endsWith" dxfId="188" priority="75" operator="endsWith" text=" of">
+    <cfRule type="endsWith" dxfId="201" priority="75" operator="endsWith" text=" of">
       <formula>RIGHT(A9,LEN(" of"))=" of"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="187" priority="76">
+    <cfRule type="expression" dxfId="200" priority="76">
       <formula>AND((RIGHT(A8, 3) = " of"), A10 = "With Properties")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="186" priority="77">
+    <cfRule type="expression" dxfId="199" priority="77">
       <formula>AND(RIGHT(XFD9, 3) = " of", A10 = "With Properties")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A9:B13">
-    <cfRule type="notContainsBlanks" dxfId="185" priority="78">
+    <cfRule type="notContainsBlanks" dxfId="198" priority="78">
       <formula>LEN(TRIM(A9))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A9:B13">
-    <cfRule type="cellIs" dxfId="184" priority="67" operator="equal">
+    <cfRule type="cellIs" dxfId="197" priority="67" operator="equal">
       <formula>"PercentagePrecision"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="183" priority="68" operator="equal">
+    <cfRule type="cellIs" dxfId="196" priority="68" operator="equal">
       <formula>"="</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A9:B13">
-    <cfRule type="cellIs" dxfId="182" priority="66" operator="equal">
+    <cfRule type="cellIs" dxfId="195" priority="66" operator="equal">
       <formula>"StringFormat"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10:D11">
-    <cfRule type="cellIs" dxfId="181" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="194" priority="56" operator="equal">
       <formula>"Assert"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="180" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="193" priority="57" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="179" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="192" priority="58" operator="equal">
       <formula>"Given a"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="178" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="191" priority="59" operator="equal">
       <formula>"Specification"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="177" priority="60" operator="beginsWith" text="With Properties">
+    <cfRule type="beginsWith" dxfId="190" priority="60" operator="beginsWith" text="With Properties">
       <formula>LEFT(D10,LEN("With Properties"))="With Properties"</formula>
     </cfRule>
-    <cfRule type="endsWith" dxfId="176" priority="61" operator="endsWith" text=" table of">
+    <cfRule type="endsWith" dxfId="189" priority="61" operator="endsWith" text=" table of">
       <formula>RIGHT(D10,LEN(" table of"))=" table of"</formula>
     </cfRule>
-    <cfRule type="endsWith" dxfId="175" priority="62" operator="endsWith" text=" of">
+    <cfRule type="endsWith" dxfId="188" priority="62" operator="endsWith" text=" of">
       <formula>RIGHT(D10,LEN(" of"))=" of"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="174" priority="63">
+    <cfRule type="expression" dxfId="187" priority="63">
       <formula>AND((RIGHT(D9, 3) = " of"), D11 = "With Properties")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="173" priority="64">
+    <cfRule type="expression" dxfId="186" priority="64">
       <formula>AND(RIGHT(C10, 3) = " of", D11 = "With Properties")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10:D11">
-    <cfRule type="notContainsBlanks" dxfId="172" priority="65">
+    <cfRule type="notContainsBlanks" dxfId="185" priority="65">
       <formula>LEN(TRIM(D10))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10:D11">
-    <cfRule type="cellIs" dxfId="171" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="184" priority="54" operator="equal">
       <formula>"PercentagePrecision"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="170" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="183" priority="55" operator="equal">
       <formula>"="</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10:D11">
-    <cfRule type="cellIs" dxfId="169" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="182" priority="53" operator="equal">
       <formula>"StringFormat"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="cellIs" dxfId="168" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="181" priority="43" operator="equal">
       <formula>"Assert"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="167" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="180" priority="44" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="166" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="179" priority="45" operator="equal">
       <formula>"Given a"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="165" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="178" priority="46" operator="equal">
       <formula>"Specification"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="164" priority="47" operator="beginsWith" text="With Properties">
+    <cfRule type="beginsWith" dxfId="177" priority="47" operator="beginsWith" text="With Properties">
       <formula>LEFT(D8,LEN("With Properties"))="With Properties"</formula>
     </cfRule>
-    <cfRule type="endsWith" dxfId="163" priority="48" operator="endsWith" text=" table of">
+    <cfRule type="endsWith" dxfId="176" priority="48" operator="endsWith" text=" table of">
       <formula>RIGHT(D8,LEN(" table of"))=" table of"</formula>
     </cfRule>
-    <cfRule type="endsWith" dxfId="162" priority="49" operator="endsWith" text=" of">
+    <cfRule type="endsWith" dxfId="175" priority="49" operator="endsWith" text=" of">
       <formula>RIGHT(D8,LEN(" of"))=" of"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="161" priority="50">
+    <cfRule type="expression" dxfId="174" priority="50">
       <formula>AND((RIGHT(D7, 3) = " of"), D9 = "With Properties")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="160" priority="51">
+    <cfRule type="expression" dxfId="173" priority="51">
       <formula>AND(RIGHT(C8, 3) = " of", D9 = "With Properties")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="notContainsBlanks" dxfId="159" priority="52">
+    <cfRule type="notContainsBlanks" dxfId="172" priority="52">
       <formula>LEN(TRIM(D8))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="cellIs" dxfId="158" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="171" priority="41" operator="equal">
       <formula>"PercentagePrecision"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="157" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="170" priority="42" operator="equal">
       <formula>"="</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="cellIs" dxfId="156" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="169" priority="40" operator="equal">
       <formula>"StringFormat"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="cellIs" dxfId="155" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="168" priority="30" operator="equal">
       <formula>"Assert"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="154" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="167" priority="31" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="153" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="166" priority="32" operator="equal">
       <formula>"Given a"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="152" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="165" priority="33" operator="equal">
       <formula>"Specification"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="151" priority="34" operator="beginsWith" text="With Properties">
+    <cfRule type="beginsWith" dxfId="164" priority="34" operator="beginsWith" text="With Properties">
       <formula>LEFT(D6,LEN("With Properties"))="With Properties"</formula>
     </cfRule>
-    <cfRule type="endsWith" dxfId="150" priority="35" operator="endsWith" text=" table of">
+    <cfRule type="endsWith" dxfId="163" priority="35" operator="endsWith" text=" table of">
       <formula>RIGHT(D6,LEN(" table of"))=" table of"</formula>
     </cfRule>
-    <cfRule type="endsWith" dxfId="149" priority="36" operator="endsWith" text=" of">
+    <cfRule type="endsWith" dxfId="162" priority="36" operator="endsWith" text=" of">
       <formula>RIGHT(D6,LEN(" of"))=" of"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="148" priority="37">
+    <cfRule type="expression" dxfId="161" priority="37">
       <formula>AND((RIGHT(D5, 3) = " of"), D7 = "With Properties")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="147" priority="38">
+    <cfRule type="expression" dxfId="160" priority="38">
       <formula>AND(RIGHT(C6, 3) = " of", D7 = "With Properties")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="notContainsBlanks" dxfId="146" priority="39">
+    <cfRule type="notContainsBlanks" dxfId="159" priority="39">
       <formula>LEN(TRIM(D6))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="cellIs" dxfId="145" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="158" priority="28" operator="equal">
       <formula>"PercentagePrecision"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="144" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="157" priority="29" operator="equal">
       <formula>"="</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="cellIs" dxfId="143" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="156" priority="27" operator="equal">
       <formula>"StringFormat"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="cellIs" dxfId="142" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="155" priority="17" operator="equal">
       <formula>"Assert"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="141" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="154" priority="18" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="140" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="153" priority="19" operator="equal">
       <formula>"Given a"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="139" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="152" priority="20" operator="equal">
       <formula>"Specification"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="138" priority="21" operator="beginsWith" text="With Properties">
+    <cfRule type="beginsWith" dxfId="151" priority="21" operator="beginsWith" text="With Properties">
       <formula>LEFT(D7,LEN("With Properties"))="With Properties"</formula>
     </cfRule>
-    <cfRule type="endsWith" dxfId="137" priority="22" operator="endsWith" text=" table of">
+    <cfRule type="endsWith" dxfId="150" priority="22" operator="endsWith" text=" table of">
       <formula>RIGHT(D7,LEN(" table of"))=" table of"</formula>
     </cfRule>
-    <cfRule type="endsWith" dxfId="136" priority="23" operator="endsWith" text=" of">
+    <cfRule type="endsWith" dxfId="149" priority="23" operator="endsWith" text=" of">
       <formula>RIGHT(D7,LEN(" of"))=" of"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="135" priority="24">
+    <cfRule type="expression" dxfId="148" priority="24">
       <formula>AND((RIGHT(D6, 3) = " of"), D8 = "With Properties")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="134" priority="25">
+    <cfRule type="expression" dxfId="147" priority="25">
       <formula>AND(RIGHT(C7, 3) = " of", D8 = "With Properties")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="notContainsBlanks" dxfId="133" priority="26">
+    <cfRule type="notContainsBlanks" dxfId="146" priority="26">
       <formula>LEN(TRIM(D7))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="cellIs" dxfId="132" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="145" priority="15" operator="equal">
       <formula>"PercentagePrecision"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="131" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="144" priority="16" operator="equal">
       <formula>"="</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="cellIs" dxfId="130" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="143" priority="14" operator="equal">
       <formula>"StringFormat"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="cellIs" dxfId="129" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="142" priority="4" operator="equal">
       <formula>"Assert"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="128" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="141" priority="5" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="127" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="140" priority="6" operator="equal">
       <formula>"Given a"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="126" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="139" priority="7" operator="equal">
       <formula>"Specification"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="125" priority="8" operator="beginsWith" text="With Properties">
+    <cfRule type="beginsWith" dxfId="138" priority="8" operator="beginsWith" text="With Properties">
       <formula>LEFT(E8,LEN("With Properties"))="With Properties"</formula>
     </cfRule>
-    <cfRule type="endsWith" dxfId="124" priority="9" operator="endsWith" text=" table of">
+    <cfRule type="endsWith" dxfId="137" priority="9" operator="endsWith" text=" table of">
       <formula>RIGHT(E8,LEN(" table of"))=" table of"</formula>
     </cfRule>
-    <cfRule type="endsWith" dxfId="123" priority="10" operator="endsWith" text=" of">
+    <cfRule type="endsWith" dxfId="136" priority="10" operator="endsWith" text=" of">
       <formula>RIGHT(E8,LEN(" of"))=" of"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="122" priority="11">
+    <cfRule type="expression" dxfId="135" priority="11">
       <formula>AND((RIGHT(E7, 3) = " of"), E9 = "With Properties")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="121" priority="12">
+    <cfRule type="expression" dxfId="134" priority="12">
       <formula>AND(RIGHT(D8, 3) = " of", E9 = "With Properties")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="notContainsBlanks" dxfId="120" priority="13">
+    <cfRule type="notContainsBlanks" dxfId="133" priority="13">
       <formula>LEN(TRIM(E8))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="cellIs" dxfId="119" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="132" priority="2" operator="equal">
       <formula>"PercentagePrecision"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="118" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="131" priority="3" operator="equal">
       <formula>"="</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="cellIs" dxfId="117" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="130" priority="1" operator="equal">
       <formula>"StringFormat"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3047,7 +3184,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -3061,7 +3198,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -3078,10 +3215,10 @@
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -3098,7 +3235,7 @@
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F7" s="1">
         <v>1</v>
@@ -3127,7 +3264,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -3183,378 +3320,378 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F1:G1">
-    <cfRule type="cellIs" dxfId="116" priority="121" operator="equal">
+    <cfRule type="cellIs" dxfId="129" priority="121" operator="equal">
       <formula>"Assert"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="115" priority="122" operator="equal">
+    <cfRule type="cellIs" dxfId="128" priority="122" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="114" priority="123" operator="equal">
+    <cfRule type="cellIs" dxfId="127" priority="123" operator="equal">
       <formula>"Given a"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="113" priority="124" operator="equal">
+    <cfRule type="cellIs" dxfId="126" priority="124" operator="equal">
       <formula>"Specification"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="112" priority="125" operator="beginsWith" text="With Properties">
+    <cfRule type="beginsWith" dxfId="125" priority="125" operator="beginsWith" text="With Properties">
       <formula>LEFT(F1,LEN("With Properties"))="With Properties"</formula>
     </cfRule>
-    <cfRule type="endsWith" dxfId="111" priority="126" operator="endsWith" text=" table of">
+    <cfRule type="endsWith" dxfId="124" priority="126" operator="endsWith" text=" table of">
       <formula>RIGHT(F1,LEN(" table of"))=" table of"</formula>
     </cfRule>
-    <cfRule type="endsWith" dxfId="110" priority="127" operator="endsWith" text=" of">
+    <cfRule type="endsWith" dxfId="123" priority="127" operator="endsWith" text=" of">
       <formula>RIGHT(F1,LEN(" of"))=" of"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="109" priority="128">
+    <cfRule type="expression" dxfId="122" priority="128">
       <formula>AND((RIGHT(F1048576, 3) = " of"), F2 = "With Properties")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="108" priority="129">
+    <cfRule type="expression" dxfId="121" priority="129">
       <formula>AND(RIGHT(E1, 3) = " of", F2 = "With Properties")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:G1">
-    <cfRule type="notContainsBlanks" dxfId="107" priority="130">
+    <cfRule type="notContainsBlanks" dxfId="120" priority="130">
       <formula>LEN(TRIM(F1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:G1">
-    <cfRule type="cellIs" dxfId="106" priority="119" operator="equal">
+    <cfRule type="cellIs" dxfId="119" priority="119" operator="equal">
       <formula>"PercentagePrecision"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="105" priority="120" operator="equal">
+    <cfRule type="cellIs" dxfId="118" priority="120" operator="equal">
       <formula>"="</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:G1">
-    <cfRule type="cellIs" dxfId="104" priority="118" operator="equal">
+    <cfRule type="cellIs" dxfId="117" priority="118" operator="equal">
       <formula>"StringFormat"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8:C8 A13:D18 A1:D7">
-    <cfRule type="cellIs" dxfId="103" priority="108" operator="equal">
+    <cfRule type="cellIs" dxfId="116" priority="108" operator="equal">
       <formula>"Assert"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="102" priority="109" operator="equal">
+    <cfRule type="cellIs" dxfId="115" priority="109" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="101" priority="110" operator="equal">
+    <cfRule type="cellIs" dxfId="114" priority="110" operator="equal">
       <formula>"Given a"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="100" priority="111" operator="equal">
+    <cfRule type="cellIs" dxfId="113" priority="111" operator="equal">
       <formula>"Specification"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="99" priority="112" operator="beginsWith" text="With Properties">
+    <cfRule type="beginsWith" dxfId="112" priority="112" operator="beginsWith" text="With Properties">
       <formula>LEFT(A1,LEN("With Properties"))="With Properties"</formula>
     </cfRule>
-    <cfRule type="endsWith" dxfId="98" priority="113" operator="endsWith" text=" table of">
+    <cfRule type="endsWith" dxfId="111" priority="113" operator="endsWith" text=" table of">
       <formula>RIGHT(A1,LEN(" table of"))=" table of"</formula>
     </cfRule>
-    <cfRule type="endsWith" dxfId="97" priority="114" operator="endsWith" text=" of">
+    <cfRule type="endsWith" dxfId="110" priority="114" operator="endsWith" text=" of">
       <formula>RIGHT(A1,LEN(" of"))=" of"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="96" priority="115">
+    <cfRule type="expression" dxfId="109" priority="115">
       <formula>AND((RIGHT(A1048576, 3) = " of"), A2 = "With Properties")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="95" priority="116">
+    <cfRule type="expression" dxfId="108" priority="116">
       <formula>AND(RIGHT(XFD1, 3) = " of", A2 = "With Properties")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8:C8 A13:D18 A1:D7">
-    <cfRule type="notContainsBlanks" dxfId="94" priority="117">
+    <cfRule type="notContainsBlanks" dxfId="107" priority="117">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8:C8 A13:D18 A1:D7">
-    <cfRule type="cellIs" dxfId="93" priority="106" operator="equal">
+    <cfRule type="cellIs" dxfId="106" priority="106" operator="equal">
       <formula>"PercentagePrecision"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="92" priority="107" operator="equal">
+    <cfRule type="cellIs" dxfId="105" priority="107" operator="equal">
       <formula>"="</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8:C8 A13:D18 A1:D7">
-    <cfRule type="cellIs" dxfId="91" priority="105" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="105" operator="equal">
       <formula>"StringFormat"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A13:B13">
-    <cfRule type="cellIs" dxfId="90" priority="82" operator="equal">
+    <cfRule type="cellIs" dxfId="103" priority="82" operator="equal">
       <formula>"Assert"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="89" priority="83" operator="equal">
+    <cfRule type="cellIs" dxfId="102" priority="83" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="88" priority="84" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="84" operator="equal">
       <formula>"Given a"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="87" priority="85" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="85" operator="equal">
       <formula>"Specification"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="86" priority="86" operator="beginsWith" text="With Properties">
+    <cfRule type="beginsWith" dxfId="99" priority="86" operator="beginsWith" text="With Properties">
       <formula>LEFT(A13,LEN("With Properties"))="With Properties"</formula>
     </cfRule>
-    <cfRule type="endsWith" dxfId="85" priority="87" operator="endsWith" text=" table of">
+    <cfRule type="endsWith" dxfId="98" priority="87" operator="endsWith" text=" table of">
       <formula>RIGHT(A13,LEN(" table of"))=" table of"</formula>
     </cfRule>
-    <cfRule type="endsWith" dxfId="84" priority="88" operator="endsWith" text=" of">
+    <cfRule type="endsWith" dxfId="97" priority="88" operator="endsWith" text=" of">
       <formula>RIGHT(A13,LEN(" of"))=" of"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="83" priority="89">
+    <cfRule type="expression" dxfId="96" priority="89">
       <formula>AND((RIGHT(A12, 3) = " of"), A14 = "With Properties")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="82" priority="90">
+    <cfRule type="expression" dxfId="95" priority="90">
       <formula>AND(RIGHT(XFD13, 3) = " of", A14 = "With Properties")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A13:B13">
-    <cfRule type="notContainsBlanks" dxfId="81" priority="91">
+    <cfRule type="notContainsBlanks" dxfId="94" priority="91">
       <formula>LEN(TRIM(A13))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A13:B13">
-    <cfRule type="cellIs" dxfId="80" priority="80" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="80" operator="equal">
       <formula>"PercentagePrecision"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="79" priority="81" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="81" operator="equal">
       <formula>"="</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A13:B13">
-    <cfRule type="cellIs" dxfId="78" priority="79" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="79" operator="equal">
       <formula>"StringFormat"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="cellIs" dxfId="77" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="90" priority="56" operator="equal">
       <formula>"Assert"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="57" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="75" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="58" operator="equal">
       <formula>"Given a"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="59" operator="equal">
       <formula>"Specification"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="73" priority="60" operator="beginsWith" text="With Properties">
+    <cfRule type="beginsWith" dxfId="86" priority="60" operator="beginsWith" text="With Properties">
       <formula>LEFT(D8,LEN("With Properties"))="With Properties"</formula>
     </cfRule>
-    <cfRule type="endsWith" dxfId="72" priority="61" operator="endsWith" text=" table of">
+    <cfRule type="endsWith" dxfId="85" priority="61" operator="endsWith" text=" table of">
       <formula>RIGHT(D8,LEN(" table of"))=" table of"</formula>
     </cfRule>
-    <cfRule type="endsWith" dxfId="71" priority="62" operator="endsWith" text=" of">
+    <cfRule type="endsWith" dxfId="84" priority="62" operator="endsWith" text=" of">
       <formula>RIGHT(D8,LEN(" of"))=" of"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="70" priority="63">
+    <cfRule type="expression" dxfId="83" priority="63">
       <formula>AND((RIGHT(D7, 3) = " of"), D9 = "With Properties")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="69" priority="64">
+    <cfRule type="expression" dxfId="82" priority="64">
       <formula>AND(RIGHT(C8, 3) = " of", D9 = "With Properties")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="notContainsBlanks" dxfId="68" priority="65">
+    <cfRule type="notContainsBlanks" dxfId="81" priority="65">
       <formula>LEN(TRIM(D8))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="cellIs" dxfId="67" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="54" operator="equal">
       <formula>"PercentagePrecision"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="55" operator="equal">
       <formula>"="</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="cellIs" dxfId="65" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="53" operator="equal">
       <formula>"StringFormat"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="cellIs" dxfId="64" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="43" operator="equal">
       <formula>"Assert"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="44" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="45" operator="equal">
       <formula>"Given a"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="46" operator="equal">
       <formula>"Specification"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="60" priority="47" operator="beginsWith" text="With Properties">
+    <cfRule type="beginsWith" dxfId="73" priority="47" operator="beginsWith" text="With Properties">
       <formula>LEFT(D6,LEN("With Properties"))="With Properties"</formula>
     </cfRule>
-    <cfRule type="endsWith" dxfId="59" priority="48" operator="endsWith" text=" table of">
+    <cfRule type="endsWith" dxfId="72" priority="48" operator="endsWith" text=" table of">
       <formula>RIGHT(D6,LEN(" table of"))=" table of"</formula>
     </cfRule>
-    <cfRule type="endsWith" dxfId="58" priority="49" operator="endsWith" text=" of">
+    <cfRule type="endsWith" dxfId="71" priority="49" operator="endsWith" text=" of">
       <formula>RIGHT(D6,LEN(" of"))=" of"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="57" priority="50">
+    <cfRule type="expression" dxfId="70" priority="50">
       <formula>AND((RIGHT(D5, 3) = " of"), D7 = "With Properties")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="56" priority="51">
+    <cfRule type="expression" dxfId="69" priority="51">
       <formula>AND(RIGHT(C6, 3) = " of", D7 = "With Properties")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="notContainsBlanks" dxfId="55" priority="52">
+    <cfRule type="notContainsBlanks" dxfId="68" priority="52">
       <formula>LEN(TRIM(D6))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="cellIs" dxfId="54" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="41" operator="equal">
       <formula>"PercentagePrecision"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="42" operator="equal">
       <formula>"="</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="cellIs" dxfId="52" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="40" operator="equal">
       <formula>"StringFormat"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="cellIs" dxfId="51" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="30" operator="equal">
       <formula>"Assert"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="31" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="32" operator="equal">
       <formula>"Given a"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="33" operator="equal">
       <formula>"Specification"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="47" priority="34" operator="beginsWith" text="With Properties">
+    <cfRule type="beginsWith" dxfId="60" priority="34" operator="beginsWith" text="With Properties">
       <formula>LEFT(D7,LEN("With Properties"))="With Properties"</formula>
     </cfRule>
-    <cfRule type="endsWith" dxfId="46" priority="35" operator="endsWith" text=" table of">
+    <cfRule type="endsWith" dxfId="59" priority="35" operator="endsWith" text=" table of">
       <formula>RIGHT(D7,LEN(" table of"))=" table of"</formula>
     </cfRule>
-    <cfRule type="endsWith" dxfId="45" priority="36" operator="endsWith" text=" of">
+    <cfRule type="endsWith" dxfId="58" priority="36" operator="endsWith" text=" of">
       <formula>RIGHT(D7,LEN(" of"))=" of"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="44" priority="37">
+    <cfRule type="expression" dxfId="57" priority="37">
       <formula>AND((RIGHT(D6, 3) = " of"), D8 = "With Properties")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="43" priority="38">
+    <cfRule type="expression" dxfId="56" priority="38">
       <formula>AND(RIGHT(C7, 3) = " of", D8 = "With Properties")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="notContainsBlanks" dxfId="42" priority="39">
+    <cfRule type="notContainsBlanks" dxfId="55" priority="39">
       <formula>LEN(TRIM(D7))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="cellIs" dxfId="41" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="28" operator="equal">
       <formula>"PercentagePrecision"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="29" operator="equal">
       <formula>"="</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="cellIs" dxfId="39" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="27" operator="equal">
       <formula>"StringFormat"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A9:D12">
-    <cfRule type="cellIs" dxfId="38" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="17" operator="equal">
       <formula>"Assert"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="18" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="19" operator="equal">
       <formula>"Given a"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="20" operator="equal">
       <formula>"Specification"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="34" priority="21" operator="beginsWith" text="With Properties">
+    <cfRule type="beginsWith" dxfId="47" priority="21" operator="beginsWith" text="With Properties">
       <formula>LEFT(A9,LEN("With Properties"))="With Properties"</formula>
     </cfRule>
-    <cfRule type="endsWith" dxfId="33" priority="22" operator="endsWith" text=" table of">
+    <cfRule type="endsWith" dxfId="46" priority="22" operator="endsWith" text=" table of">
       <formula>RIGHT(A9,LEN(" table of"))=" table of"</formula>
     </cfRule>
-    <cfRule type="endsWith" dxfId="32" priority="23" operator="endsWith" text=" of">
+    <cfRule type="endsWith" dxfId="45" priority="23" operator="endsWith" text=" of">
       <formula>RIGHT(A9,LEN(" of"))=" of"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="24">
+    <cfRule type="expression" dxfId="44" priority="24">
       <formula>AND((RIGHT(A8, 3) = " of"), A10 = "With Properties")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="25">
+    <cfRule type="expression" dxfId="43" priority="25">
       <formula>AND(RIGHT(XFD9, 3) = " of", A10 = "With Properties")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A9:D12">
-    <cfRule type="notContainsBlanks" dxfId="29" priority="26">
+    <cfRule type="notContainsBlanks" dxfId="42" priority="26">
       <formula>LEN(TRIM(A9))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A9:D12">
-    <cfRule type="cellIs" dxfId="28" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="15" operator="equal">
       <formula>"PercentagePrecision"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="16" operator="equal">
       <formula>"="</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A9:D12">
-    <cfRule type="cellIs" dxfId="26" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="14" operator="equal">
       <formula>"StringFormat"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7:F7">
-    <cfRule type="cellIs" dxfId="25" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="4" operator="equal">
       <formula>"Assert"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="5" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="6" operator="equal">
       <formula>"Given a"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="7" operator="equal">
       <formula>"Specification"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="21" priority="8" operator="beginsWith" text="With Properties">
+    <cfRule type="beginsWith" dxfId="34" priority="8" operator="beginsWith" text="With Properties">
       <formula>LEFT(E7,LEN("With Properties"))="With Properties"</formula>
     </cfRule>
-    <cfRule type="endsWith" dxfId="20" priority="9" operator="endsWith" text=" table of">
+    <cfRule type="endsWith" dxfId="33" priority="9" operator="endsWith" text=" table of">
       <formula>RIGHT(E7,LEN(" table of"))=" table of"</formula>
     </cfRule>
-    <cfRule type="endsWith" dxfId="19" priority="10" operator="endsWith" text=" of">
+    <cfRule type="endsWith" dxfId="32" priority="10" operator="endsWith" text=" of">
       <formula>RIGHT(E7,LEN(" of"))=" of"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="11">
+    <cfRule type="expression" dxfId="31" priority="11">
       <formula>AND((RIGHT(E6, 3) = " of"), E8 = "With Properties")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="12">
+    <cfRule type="expression" dxfId="30" priority="12">
       <formula>AND(RIGHT(D7, 3) = " of", E8 = "With Properties")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7:F7">
-    <cfRule type="notContainsBlanks" dxfId="16" priority="13">
+    <cfRule type="notContainsBlanks" dxfId="29" priority="13">
       <formula>LEN(TRIM(E7))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7:F7">
-    <cfRule type="cellIs" dxfId="15" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="2" operator="equal">
       <formula>"PercentagePrecision"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="3" operator="equal">
       <formula>"="</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7:F7">
-    <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="1" operator="equal">
       <formula>"StringFormat"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3566,8 +3703,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B439CE3-5D92-415D-93E7-26C8C7404B89}">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3579,7 +3716,8 @@
     <col min="5" max="5" width="20.7109375" style="3" customWidth="1"/>
     <col min="6" max="6" width="15.5703125" style="3" customWidth="1"/>
     <col min="7" max="7" width="22.5703125" style="3" customWidth="1"/>
-    <col min="8" max="9" width="9.140625" style="3"/>
+    <col min="8" max="8" width="79.5703125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="3"/>
     <col min="10" max="10" width="71.28515625" style="3" customWidth="1"/>
     <col min="11" max="16384" width="9.140625" style="3"/>
   </cols>
@@ -3589,7 +3727,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -3598,7 +3736,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H1" s="1"/>
     </row>
@@ -3617,7 +3755,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -3638,60 +3776,58 @@
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
-      <c r="J5" s="1" t="s">
-        <v>39</v>
-      </c>
+      <c r="J5" s="1"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
+      <c r="C6" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="D6" s="1" t="s">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>37</v>
-      </c>
+      <c r="D7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
-      <c r="J7" s="1" t="s">
-        <v>39</v>
-      </c>
+      <c r="J7" s="1"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
+      <c r="E8" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="F8" s="1" t="s">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
@@ -3700,46 +3836,42 @@
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
+      <c r="D9" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
-      <c r="G9" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="H9" s="1">
-        <v>1</v>
-      </c>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
+      <c r="A10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>31</v>
-      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
-      <c r="C11" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>31</v>
-      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
+      <c r="A12" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -3749,14 +3881,16 @@
       <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
+        <v>9</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="1">
+        <v>1</v>
+      </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
@@ -3773,9 +3907,7 @@
       <c r="H14" s="1"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -3786,15 +3918,9 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
-      <c r="B16" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D16" s="1">
-        <v>1</v>
-      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
@@ -3811,7 +3937,195 @@
       <c r="H17" s="1"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:H17">
+  <conditionalFormatting sqref="A9:H17 A8:G8 D6:F8 A1:H5 A7:H7 A6:G6">
+    <cfRule type="cellIs" dxfId="25" priority="4" operator="equal">
+      <formula>"Assert"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="5" operator="equal">
+      <formula>"When"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="23" priority="6" operator="equal">
+      <formula>"Given a"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="7" operator="equal">
+      <formula>"Specification"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="21" priority="8" operator="beginsWith" text="With Properties">
+      <formula>LEFT(A1,LEN("With Properties"))="With Properties"</formula>
+    </cfRule>
+    <cfRule type="endsWith" dxfId="20" priority="9" operator="endsWith" text=" table of">
+      <formula>RIGHT(A1,LEN(" table of"))=" table of"</formula>
+    </cfRule>
+    <cfRule type="endsWith" dxfId="19" priority="10" operator="endsWith" text=" of">
+      <formula>RIGHT(A1,LEN(" of"))=" of"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="18" priority="11">
+      <formula>AND((RIGHT(A1048576, 3) = " of"), A2 = "With Properties")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="17" priority="12">
+      <formula>AND(RIGHT(XFD1, 3) = " of", A2 = "With Properties")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A9:H17 A8:G8 D6:F8 A1:H5 A7:H7 A6:G6">
+    <cfRule type="notContainsBlanks" dxfId="16" priority="13">
+      <formula>LEN(TRIM(A1))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A9:H17 A8:G8 D6:F8 A1:H5 A7:H7 A6:G6">
+    <cfRule type="cellIs" dxfId="15" priority="2" operator="equal">
+      <formula>"PercentagePrecision"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="3" operator="equal">
+      <formula>"="</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A9:H17 A8:G8 D6:F8 A1:H5 A7:H7 A6:G6">
+    <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
+      <formula>"StringFormat"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B77C5D5-B891-4358-8ACF-858C937CAD76}">
+  <dimension ref="A1:G14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="76.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="F2" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="3"/>
+    </row>
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G5" s="3"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" s="3"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C7" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" s="1">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G7" s="3"/>
+    </row>
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G8" s="3"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="1">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A2:E9 H1:H9 A10:H16 A1:D1">
     <cfRule type="cellIs" dxfId="12" priority="4" operator="equal">
       <formula>"Assert"</formula>
     </cfRule>
@@ -3840,12 +4154,12 @@
       <formula>AND(RIGHT(XFD1, 3) = " of", A2 = "With Properties")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:H17">
+  <conditionalFormatting sqref="A2:E9 H1:H9 A10:H16 A1:D1">
     <cfRule type="notContainsBlanks" dxfId="3" priority="13">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:H17">
+  <conditionalFormatting sqref="A2:E9 H1:H9 A10:H16 A1:D1">
     <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"PercentagePrecision"</formula>
     </cfRule>
@@ -3853,7 +4167,7 @@
       <formula>"="</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:H17">
+  <conditionalFormatting sqref="A2:E9 H1:H9 A10:H16 A1:D1">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"StringFormat"</formula>
     </cfRule>

</xml_diff>